<commit_message>
Finish ryi-thankyou page bike list checking. testing usage: pytest proj12_ryi/test_case/m1201_booking_process.py.
</commit_message>
<xml_diff>
--- a/proj12_ryi/data/MY20-RYI-Matrix-V3.1.xlsx
+++ b/proj12_ryi/data/MY20-RYI-Matrix-V3.1.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel.proctor/Documents/MY20/Matrix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\bitbucket\hd-emea-test-script\proj12_ryi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA93055-E835-4D42-8875-A6AE7F0EE698}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33300" windowHeight="20540" xr2:uid="{81222261-910D-4D7E-B6ED-D92B6F28E0FE}"/>
+    <workbookView xWindow="-33600" yWindow="465" windowWidth="33300" windowHeight="20535"/>
   </bookViews>
   <sheets>
     <sheet name="RYI" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" calcMode="manual" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="309">
   <si>
     <t>Region</t>
   </si>
@@ -938,12 +937,33 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>FXBB</t>
+  </si>
+  <si>
+    <t>FLFB</t>
+  </si>
+  <si>
+    <t>FLSB</t>
+  </si>
+  <si>
+    <t>FLSL</t>
+  </si>
+  <si>
+    <t>FLDE</t>
+  </si>
+  <si>
+    <t>FXFB</t>
+  </si>
+  <si>
+    <t>FXBR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -1645,7 +1665,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{0BA4DD4C-70F9-E148-9C03-46841906C1F6}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1971,58 +1991,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CA675B-D166-4D53-BE3D-19AF26AC0D0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="J13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="5"/>
+    <col min="1" max="1" width="11.125" style="5"/>
     <col min="2" max="2" width="47.5" style="9" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="5" customWidth="1"/>
-    <col min="5" max="6" width="17.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="51.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="53.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="5" customWidth="1"/>
+    <col min="5" max="6" width="17.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20.125" style="5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="51.125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="53.375" style="5" customWidth="1"/>
     <col min="10" max="10" width="18.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="19.625" style="5" customWidth="1"/>
     <col min="12" max="13" width="18.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="19.625" style="5" customWidth="1"/>
     <col min="15" max="16" width="18.5" style="5" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="19.875" style="5" customWidth="1"/>
     <col min="18" max="18" width="18.5" style="5" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="19.625" style="5" customWidth="1"/>
     <col min="20" max="20" width="18.5" style="5" customWidth="1"/>
-    <col min="21" max="21" width="57.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="57.625" style="26" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="65" style="26" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="50.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="63.1640625" style="12" customWidth="1"/>
-    <col min="25" max="16384" width="11.1640625" style="5"/>
+    <col min="23" max="23" width="50.375" style="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="63.125" style="12" customWidth="1"/>
+    <col min="25" max="16384" width="11.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" ht="16.5" thickBot="1">
       <c r="A1" s="10" t="s">
         <v>274</v>
       </c>
       <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="J1" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>7</v>
+      </c>
       <c r="X1" s="25"/>
     </row>
     <row r="2" spans="1:24">
@@ -2047,7 +2089,7 @@
       <c r="S2" s="95"/>
       <c r="T2" s="95"/>
     </row>
-    <row r="3" spans="1:24" s="2" customFormat="1" ht="18" thickBot="1">
+    <row r="3" spans="1:24" s="2" customFormat="1" ht="16.5" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2163,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="17">
+    <row r="4" spans="1:24">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2235,7 @@
       </c>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="17">
+    <row r="5" spans="1:24">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -2265,7 +2307,7 @@
       </c>
       <c r="X5" s="14"/>
     </row>
-    <row r="6" spans="1:24" ht="17">
+    <row r="6" spans="1:24">
       <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
@@ -2337,7 +2379,7 @@
       </c>
       <c r="X6" s="14"/>
     </row>
-    <row r="7" spans="1:24" ht="17">
+    <row r="7" spans="1:24">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -2409,7 +2451,7 @@
       </c>
       <c r="X7" s="15"/>
     </row>
-    <row r="8" spans="1:24" ht="18" thickBot="1">
+    <row r="8" spans="1:24" ht="16.5" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
@@ -2479,7 +2521,7 @@
       <c r="W8" s="66"/>
       <c r="X8" s="15"/>
     </row>
-    <row r="9" spans="1:24" ht="17">
+    <row r="9" spans="1:24">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -2549,7 +2591,7 @@
       <c r="W9" s="68"/>
       <c r="X9" s="15"/>
     </row>
-    <row r="10" spans="1:24" ht="17">
+    <row r="10" spans="1:24">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
@@ -2619,7 +2661,7 @@
       <c r="W10" s="68"/>
       <c r="X10" s="15"/>
     </row>
-    <row r="11" spans="1:24" ht="17">
+    <row r="11" spans="1:24">
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
@@ -2689,7 +2731,7 @@
       <c r="W11" s="68"/>
       <c r="X11" s="15"/>
     </row>
-    <row r="12" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="12" spans="1:24" s="8" customFormat="1">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
@@ -2759,7 +2801,7 @@
       <c r="W12" s="68"/>
       <c r="X12" s="14"/>
     </row>
-    <row r="13" spans="1:24" ht="17">
+    <row r="13" spans="1:24">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
@@ -2829,7 +2871,7 @@
       <c r="W13" s="68"/>
       <c r="X13" s="14"/>
     </row>
-    <row r="14" spans="1:24" ht="17">
+    <row r="14" spans="1:24">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -2901,7 +2943,7 @@
       </c>
       <c r="X14" s="14"/>
     </row>
-    <row r="15" spans="1:24" ht="17">
+    <row r="15" spans="1:24">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
@@ -2969,7 +3011,7 @@
       <c r="W15" s="68"/>
       <c r="X15" s="14"/>
     </row>
-    <row r="16" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="16" spans="1:24" s="8" customFormat="1">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -3039,7 +3081,7 @@
       <c r="W16" s="68"/>
       <c r="X16" s="14"/>
     </row>
-    <row r="17" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="17" spans="1:24" s="8" customFormat="1">
       <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
@@ -3109,7 +3151,7 @@
       <c r="W17" s="68"/>
       <c r="X17" s="14"/>
     </row>
-    <row r="18" spans="1:24" ht="17">
+    <row r="18" spans="1:24">
       <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
@@ -3179,7 +3221,7 @@
       <c r="W18" s="68"/>
       <c r="X18" s="14"/>
     </row>
-    <row r="19" spans="1:24" ht="17">
+    <row r="19" spans="1:24">
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
@@ -3251,7 +3293,7 @@
       </c>
       <c r="X19" s="14"/>
     </row>
-    <row r="20" spans="1:24" ht="17">
+    <row r="20" spans="1:24">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -3323,7 +3365,7 @@
       </c>
       <c r="X20" s="14"/>
     </row>
-    <row r="21" spans="1:24" ht="17">
+    <row r="21" spans="1:24">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -3391,7 +3433,7 @@
       <c r="W21" s="68"/>
       <c r="X21" s="14"/>
     </row>
-    <row r="22" spans="1:24" ht="17" customHeight="1">
+    <row r="22" spans="1:24" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
@@ -3463,7 +3505,7 @@
       </c>
       <c r="X22" s="14"/>
     </row>
-    <row r="23" spans="1:24" ht="17">
+    <row r="23" spans="1:24">
       <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
@@ -3533,7 +3575,7 @@
       <c r="W23" s="68"/>
       <c r="X23" s="14"/>
     </row>
-    <row r="24" spans="1:24" ht="17">
+    <row r="24" spans="1:24">
       <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
@@ -3605,7 +3647,7 @@
       </c>
       <c r="X24" s="14"/>
     </row>
-    <row r="25" spans="1:24" ht="17">
+    <row r="25" spans="1:24">
       <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
@@ -3677,7 +3719,7 @@
       </c>
       <c r="X25" s="14"/>
     </row>
-    <row r="26" spans="1:24" ht="17">
+    <row r="26" spans="1:24">
       <c r="A26" s="6" t="s">
         <v>27</v>
       </c>
@@ -3745,7 +3787,7 @@
       <c r="W26" s="68"/>
       <c r="X26" s="14"/>
     </row>
-    <row r="27" spans="1:24" ht="17">
+    <row r="27" spans="1:24">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
@@ -3815,7 +3857,7 @@
       <c r="W27" s="68"/>
       <c r="X27" s="14"/>
     </row>
-    <row r="28" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="28" spans="1:24" s="8" customFormat="1">
       <c r="A28" s="6" t="s">
         <v>27</v>
       </c>
@@ -3887,7 +3929,7 @@
       </c>
       <c r="X28" s="16"/>
     </row>
-    <row r="29" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="29" spans="1:24" s="8" customFormat="1">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -3959,7 +4001,7 @@
       </c>
       <c r="X29" s="14"/>
     </row>
-    <row r="30" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="30" spans="1:24" s="8" customFormat="1">
       <c r="A30" s="6" t="s">
         <v>27</v>
       </c>
@@ -4031,7 +4073,7 @@
       </c>
       <c r="X30" s="14"/>
     </row>
-    <row r="31" spans="1:24" ht="17">
+    <row r="31" spans="1:24">
       <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
@@ -4103,7 +4145,7 @@
       </c>
       <c r="X31" s="14"/>
     </row>
-    <row r="32" spans="1:24" ht="17">
+    <row r="32" spans="1:24">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -4173,7 +4215,7 @@
       <c r="W32" s="68"/>
       <c r="X32" s="14"/>
     </row>
-    <row r="33" spans="1:24" ht="17">
+    <row r="33" spans="1:24">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4245,7 +4287,7 @@
       </c>
       <c r="X33" s="14"/>
     </row>
-    <row r="34" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="34" spans="1:24" s="8" customFormat="1">
       <c r="A34" s="6" t="s">
         <v>27</v>
       </c>
@@ -4315,7 +4357,7 @@
       <c r="W34" s="68"/>
       <c r="X34" s="14"/>
     </row>
-    <row r="35" spans="1:24" ht="17">
+    <row r="35" spans="1:24">
       <c r="A35" s="6" t="s">
         <v>27</v>
       </c>
@@ -4383,7 +4425,7 @@
       <c r="W35" s="63"/>
       <c r="X35" s="14"/>
     </row>
-    <row r="36" spans="1:24" ht="17" thickBot="1">
+    <row r="36" spans="1:24" ht="16.5" thickBot="1">
       <c r="A36" s="18" t="s">
         <v>27</v>
       </c>
@@ -4449,7 +4491,7 @@
       <c r="W36" s="70"/>
       <c r="X36" s="22"/>
     </row>
-    <row r="37" spans="1:24" ht="18" thickBot="1">
+    <row r="37" spans="1:24" ht="16.5" thickBot="1">
       <c r="A37" s="29" t="s">
         <v>17</v>
       </c>
@@ -4515,7 +4557,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="17">
+    <row r="38" spans="1:24">
       <c r="A38" s="32" t="s">
         <v>17</v>
       </c>
@@ -4579,7 +4621,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="17">
+    <row r="39" spans="1:24">
       <c r="A39" s="37" t="s">
         <v>17</v>
       </c>
@@ -4643,7 +4685,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="17">
+    <row r="40" spans="1:24">
       <c r="A40" s="37" t="s">
         <v>17</v>
       </c>
@@ -4707,7 +4749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="17">
+    <row r="41" spans="1:24">
       <c r="A41" s="37" t="s">
         <v>17</v>
       </c>
@@ -4771,7 +4813,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="17">
+    <row r="42" spans="1:24">
       <c r="A42" s="37" t="s">
         <v>17</v>
       </c>
@@ -4835,7 +4877,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="17">
+    <row r="43" spans="1:24">
       <c r="A43" s="37" t="s">
         <v>17</v>
       </c>
@@ -4899,7 +4941,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="17">
+    <row r="44" spans="1:24">
       <c r="A44" s="37" t="s">
         <v>17</v>
       </c>
@@ -4963,7 +5005,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="17">
+    <row r="45" spans="1:24">
       <c r="A45" s="37" t="s">
         <v>17</v>
       </c>
@@ -5027,7 +5069,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:24" s="8" customFormat="1" ht="17">
+    <row r="46" spans="1:24" s="8" customFormat="1">
       <c r="A46" s="37" t="s">
         <v>17</v>
       </c>
@@ -5091,7 +5133,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="18" thickBot="1">
+    <row r="47" spans="1:24" ht="16.5" thickBot="1">
       <c r="A47" s="41" t="s">
         <v>17</v>
       </c>
@@ -5168,77 +5210,77 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{15CAEFFB-FE73-474A-90BF-1431BB2FC28A}"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://h-d.com/ridefree" xr:uid="{07A9B565-5B0A-4270-9FA1-B845B84E7AE7}"/>
-    <hyperlink ref="U8" r:id="rId3" xr:uid="{EF6064C8-B19B-BD48-A87B-BB0ECB3407B0}"/>
-    <hyperlink ref="U6" r:id="rId4" xr:uid="{C7080D0C-E7C6-A84F-8EAD-B72769E21772}"/>
-    <hyperlink ref="U5" r:id="rId5" xr:uid="{19F5B714-4C74-BD42-BB16-CA05BDBC2D50}"/>
-    <hyperlink ref="U16" r:id="rId6" xr:uid="{282E26F9-11BE-524A-A320-F3D77EAA7B5E}"/>
-    <hyperlink ref="U18" r:id="rId7" xr:uid="{05DDD474-972E-9642-B769-8EFD0B3CEDB9}"/>
-    <hyperlink ref="U24" r:id="rId8" xr:uid="{C9C5931E-D872-2A4E-BA4D-F4BAAFE8235C}"/>
-    <hyperlink ref="U14" r:id="rId9" xr:uid="{E139ADB2-4CDA-294C-9113-A264AD6A8E1D}"/>
-    <hyperlink ref="U20" r:id="rId10" xr:uid="{B1564D91-682F-5247-BA42-06A85DD9F11B}"/>
-    <hyperlink ref="U33" r:id="rId11" xr:uid="{3C85310E-A423-0042-B8F6-8C541B55671B}"/>
-    <hyperlink ref="U28" r:id="rId12" xr:uid="{BD7154C4-1D98-C941-9E70-4BE1EE714B03}"/>
-    <hyperlink ref="U4" r:id="rId13" xr:uid="{9AE079FA-FD92-C14D-88AD-5E9F2A947152}"/>
-    <hyperlink ref="U7" r:id="rId14" xr:uid="{91CF9305-369F-1B4D-96A9-F7507577A08A}"/>
-    <hyperlink ref="U11" r:id="rId15" xr:uid="{3DE2967C-0BDE-A04A-A12F-2E796920BADF}"/>
-    <hyperlink ref="U13" r:id="rId16" xr:uid="{8333CCE8-3B98-4D49-9133-7ED8F43857C4}"/>
-    <hyperlink ref="U23" r:id="rId17" xr:uid="{74297967-A4CB-6041-97AA-356531242BA0}"/>
-    <hyperlink ref="U27" r:id="rId18" xr:uid="{C427E11B-5AFB-3246-AB95-777E7AEDBDAA}"/>
-    <hyperlink ref="U12" r:id="rId19" xr:uid="{6DF3D114-F5A0-0841-BAF6-F0E0DE1D2FFB}"/>
-    <hyperlink ref="U22" r:id="rId20" xr:uid="{E091F799-6614-3048-BD1E-1D5ED1D867C5}"/>
-    <hyperlink ref="U29" r:id="rId21" xr:uid="{B3431089-81AD-8B4F-AD40-F38CC79C1F48}"/>
-    <hyperlink ref="U25" r:id="rId22" xr:uid="{E1CC1211-45FC-274A-A6B5-FEB5B869981A}"/>
-    <hyperlink ref="U30" r:id="rId23" xr:uid="{5424EB50-67BD-8841-AB6D-A67ED1B4E3E8}"/>
-    <hyperlink ref="U26" r:id="rId24" xr:uid="{4DB8499B-BD69-F041-8B18-E8B076404A57}"/>
-    <hyperlink ref="U9" r:id="rId25" xr:uid="{FDA50C60-C4F4-154B-9A06-069707FA5229}"/>
-    <hyperlink ref="U32" r:id="rId26" xr:uid="{F5255D16-C1EE-A746-B7F0-EB48242E4B5E}"/>
-    <hyperlink ref="U34" r:id="rId27" xr:uid="{104AA062-3E96-0248-89E9-460A0F11D57B}"/>
-    <hyperlink ref="V8" r:id="rId28" xr:uid="{4DE9C324-64B8-344A-9424-E6CF36122D97}"/>
-    <hyperlink ref="V5" r:id="rId29" xr:uid="{44A2BD75-5A1E-4043-829B-C12130DDEA16}"/>
-    <hyperlink ref="V16" r:id="rId30" xr:uid="{95949260-3A39-8044-9436-748F7E9A6FF5}"/>
-    <hyperlink ref="V18" r:id="rId31" xr:uid="{E475A729-97EB-1E4F-B7CE-CE75B70D8F6F}"/>
-    <hyperlink ref="V24" r:id="rId32" xr:uid="{9B6F4D84-C314-264C-A6EA-6F254E9D5065}"/>
-    <hyperlink ref="V14" r:id="rId33" xr:uid="{9D8AD2D1-E160-8C46-9EBA-EC4F5BD22524}"/>
-    <hyperlink ref="V20" r:id="rId34" xr:uid="{3230E5DB-3FCF-D142-AB36-E95249DFE35F}"/>
-    <hyperlink ref="V33" r:id="rId35" xr:uid="{A0C9096C-5835-C94B-88C7-7C105A548130}"/>
-    <hyperlink ref="V28" r:id="rId36" xr:uid="{D10945C6-8CA9-734E-9EA0-4D3929A1CE95}"/>
-    <hyperlink ref="V4" r:id="rId37" xr:uid="{60A955B3-00C5-C243-A51B-F6C6C193F4DA}"/>
-    <hyperlink ref="V7" r:id="rId38" xr:uid="{4BCD44BB-247B-D74D-85BC-B85124A07DDD}"/>
-    <hyperlink ref="V11" r:id="rId39" xr:uid="{D2D67F86-7C40-AF43-B0F5-4390A16C3D06}"/>
-    <hyperlink ref="V13" r:id="rId40" xr:uid="{03AD3472-D569-D34D-B041-89D7B742ED54}"/>
-    <hyperlink ref="V23" r:id="rId41" xr:uid="{6E64A97C-064B-A440-B088-197855DE889D}"/>
-    <hyperlink ref="V27" r:id="rId42" xr:uid="{E7103C52-F09B-4240-B83E-E96E004DAAB0}"/>
-    <hyperlink ref="V12" r:id="rId43" xr:uid="{6AFCE97D-82B3-7041-B5F9-24C95D5B6C01}"/>
-    <hyperlink ref="V22" r:id="rId44" xr:uid="{8E7FAA0E-20EC-C34D-AA6D-4C7BE620A99E}"/>
-    <hyperlink ref="V29" r:id="rId45" xr:uid="{A9CCAE5E-7FD8-1540-B506-73F03E4DBA83}"/>
-    <hyperlink ref="V25" r:id="rId46" xr:uid="{0C9E7B1B-3B1C-904C-8278-6B9BFA2CFC28}"/>
-    <hyperlink ref="V30" r:id="rId47" xr:uid="{1DB5816E-E083-6446-8F3A-E7604B3C540F}"/>
-    <hyperlink ref="V34" r:id="rId48" xr:uid="{C359EDDD-B884-7A40-B812-453CB9EA7F25}"/>
-    <hyperlink ref="W5" r:id="rId49" xr:uid="{1899024B-4439-AD46-B6E9-55035FDEFF88}"/>
-    <hyperlink ref="W14" r:id="rId50" xr:uid="{A75B153E-8697-4048-B11C-680451A69EA8}"/>
-    <hyperlink ref="W24" r:id="rId51" xr:uid="{41EA4920-2860-DA4E-9136-2F0F3C89C24D}"/>
-    <hyperlink ref="W20" r:id="rId52" xr:uid="{496ABC2F-F690-FC4C-B924-C6FE93615FDC}"/>
-    <hyperlink ref="W33" r:id="rId53" xr:uid="{B556D5C6-FEFA-7847-96C7-8C27EFA83F4F}"/>
-    <hyperlink ref="W28" r:id="rId54" xr:uid="{A4B49039-93A8-8E42-BC6D-9AE28A694A35}"/>
-    <hyperlink ref="W4" r:id="rId55" xr:uid="{3B6C69F1-7E4C-AC4A-B8FF-019EC2A31E78}"/>
-    <hyperlink ref="W7" r:id="rId56" xr:uid="{D7F99017-E8FF-8949-88C5-226A527311CD}"/>
-    <hyperlink ref="W22" r:id="rId57" xr:uid="{AFE3603B-4B04-3946-AE30-9959858F3A52}"/>
-    <hyperlink ref="W29" r:id="rId58" xr:uid="{CD884E3A-5064-944E-8D24-E70DB0110950}"/>
-    <hyperlink ref="W25" r:id="rId59" xr:uid="{452927A7-82FE-6448-8A52-BA8075DEC72D}"/>
-    <hyperlink ref="W30" r:id="rId60" xr:uid="{0EF14279-4B72-D140-B624-DA7415358BE6}"/>
-    <hyperlink ref="V9" r:id="rId61" xr:uid="{1E1C815A-503D-734C-94B8-EED5EA4F6F83}"/>
-    <hyperlink ref="V32" r:id="rId62" xr:uid="{17888FA1-5B34-8E40-B2C5-5954ACB16123}"/>
-    <hyperlink ref="V17" r:id="rId63" xr:uid="{7E2AE9C0-8CFD-8F46-AFC7-F7F78AB13107}"/>
-    <hyperlink ref="U35" r:id="rId64" xr:uid="{3789C613-E12E-B644-AA9E-DDC85022B87C}"/>
-    <hyperlink ref="W31" r:id="rId65" xr:uid="{D7016F21-9096-144C-A789-DFEE6DA4C19A}"/>
-    <hyperlink ref="U31" r:id="rId66" xr:uid="{D822ED4B-0B3C-774F-8EC1-1E8A426C279C}"/>
-    <hyperlink ref="V31" r:id="rId67" xr:uid="{E6776F7F-5CC2-7544-825A-8FFBB7BDB3E6}"/>
-    <hyperlink ref="U21" r:id="rId68" xr:uid="{A686C5AE-95A6-3F4A-8482-7DB47BEC6381}"/>
-    <hyperlink ref="U10" r:id="rId69" xr:uid="{F8AFC3EC-2D59-B342-8B6E-4E362F3AC31D}"/>
-    <hyperlink ref="V10" r:id="rId70" xr:uid="{E16761DB-DDD1-7741-9DD3-4674D3E3680C}"/>
-    <hyperlink ref="H38" r:id="rId71" xr:uid="{4B76DC30-7C5A-4494-8E6F-ECE6E4D149C8}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2" display="http://h-d.com/ridefree"/>
+    <hyperlink ref="U8" r:id="rId3"/>
+    <hyperlink ref="U6" r:id="rId4"/>
+    <hyperlink ref="U5" r:id="rId5"/>
+    <hyperlink ref="U16" r:id="rId6"/>
+    <hyperlink ref="U18" r:id="rId7"/>
+    <hyperlink ref="U24" r:id="rId8"/>
+    <hyperlink ref="U14" r:id="rId9"/>
+    <hyperlink ref="U20" r:id="rId10"/>
+    <hyperlink ref="U33" r:id="rId11"/>
+    <hyperlink ref="U28" r:id="rId12"/>
+    <hyperlink ref="U4" r:id="rId13"/>
+    <hyperlink ref="U7" r:id="rId14"/>
+    <hyperlink ref="U11" r:id="rId15"/>
+    <hyperlink ref="U13" r:id="rId16"/>
+    <hyperlink ref="U23" r:id="rId17"/>
+    <hyperlink ref="U27" r:id="rId18"/>
+    <hyperlink ref="U12" r:id="rId19"/>
+    <hyperlink ref="U22" r:id="rId20"/>
+    <hyperlink ref="U29" r:id="rId21"/>
+    <hyperlink ref="U25" r:id="rId22"/>
+    <hyperlink ref="U30" r:id="rId23"/>
+    <hyperlink ref="U26" r:id="rId24"/>
+    <hyperlink ref="U9" r:id="rId25"/>
+    <hyperlink ref="U32" r:id="rId26"/>
+    <hyperlink ref="U34" r:id="rId27"/>
+    <hyperlink ref="V8" r:id="rId28"/>
+    <hyperlink ref="V5" r:id="rId29"/>
+    <hyperlink ref="V16" r:id="rId30"/>
+    <hyperlink ref="V18" r:id="rId31"/>
+    <hyperlink ref="V24" r:id="rId32"/>
+    <hyperlink ref="V14" r:id="rId33"/>
+    <hyperlink ref="V20" r:id="rId34"/>
+    <hyperlink ref="V33" r:id="rId35"/>
+    <hyperlink ref="V28" r:id="rId36"/>
+    <hyperlink ref="V4" r:id="rId37"/>
+    <hyperlink ref="V7" r:id="rId38"/>
+    <hyperlink ref="V11" r:id="rId39"/>
+    <hyperlink ref="V13" r:id="rId40"/>
+    <hyperlink ref="V23" r:id="rId41"/>
+    <hyperlink ref="V27" r:id="rId42"/>
+    <hyperlink ref="V12" r:id="rId43"/>
+    <hyperlink ref="V22" r:id="rId44"/>
+    <hyperlink ref="V29" r:id="rId45"/>
+    <hyperlink ref="V25" r:id="rId46"/>
+    <hyperlink ref="V30" r:id="rId47"/>
+    <hyperlink ref="V34" r:id="rId48"/>
+    <hyperlink ref="W5" r:id="rId49"/>
+    <hyperlink ref="W14" r:id="rId50"/>
+    <hyperlink ref="W24" r:id="rId51"/>
+    <hyperlink ref="W20" r:id="rId52"/>
+    <hyperlink ref="W33" r:id="rId53"/>
+    <hyperlink ref="W28" r:id="rId54"/>
+    <hyperlink ref="W4" r:id="rId55"/>
+    <hyperlink ref="W7" r:id="rId56"/>
+    <hyperlink ref="W22" r:id="rId57"/>
+    <hyperlink ref="W29" r:id="rId58"/>
+    <hyperlink ref="W25" r:id="rId59"/>
+    <hyperlink ref="W30" r:id="rId60"/>
+    <hyperlink ref="V9" r:id="rId61"/>
+    <hyperlink ref="V32" r:id="rId62"/>
+    <hyperlink ref="V17" r:id="rId63"/>
+    <hyperlink ref="U35" r:id="rId64"/>
+    <hyperlink ref="W31" r:id="rId65"/>
+    <hyperlink ref="U31" r:id="rId66"/>
+    <hyperlink ref="V31" r:id="rId67"/>
+    <hyperlink ref="U21" r:id="rId68"/>
+    <hyperlink ref="U10" r:id="rId69"/>
+    <hyperlink ref="V10" r:id="rId70"/>
+    <hyperlink ref="H38" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId72"/>
@@ -5246,26 +5288,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA677C9F-9278-6B42-9334-F33C0BFBAF2B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O1:Y60"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="15" max="15" width="50.83203125" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
-    <col min="20" max="20" width="3.83203125" customWidth="1"/>
-    <col min="21" max="21" width="21.1640625" customWidth="1"/>
+    <col min="15" max="15" width="50.875" customWidth="1"/>
+    <col min="19" max="19" width="16.625" customWidth="1"/>
+    <col min="20" max="20" width="3.875" customWidth="1"/>
+    <col min="21" max="21" width="21.125" customWidth="1"/>
     <col min="22" max="22" width="17.5" customWidth="1"/>
-    <col min="23" max="23" width="17.1640625" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" customWidth="1"/>
+    <col min="23" max="23" width="17.125" customWidth="1"/>
+    <col min="25" max="25" width="16.625" customWidth="1"/>
     <col min="26" max="34" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="15:25" ht="17">
+    <row r="1" spans="15:25">
       <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
@@ -5285,7 +5327,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="15:25" ht="17">
+    <row r="2" spans="15:25">
       <c r="O2" s="7" t="s">
         <v>13</v>
       </c>
@@ -5309,7 +5351,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="15:25" ht="17">
+    <row r="3" spans="15:25">
       <c r="O3" s="7" t="s">
         <v>14</v>
       </c>
@@ -5333,7 +5375,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="15:25" ht="17">
+    <row r="4" spans="15:25">
       <c r="O4" s="7" t="s">
         <v>15</v>
       </c>
@@ -5357,7 +5399,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="15:25" ht="18" thickBot="1">
+    <row r="5" spans="15:25" ht="16.5" thickBot="1">
       <c r="O5" s="19" t="s">
         <v>16</v>
       </c>
@@ -5381,7 +5423,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="15:25" ht="34">
+    <row r="6" spans="15:25" ht="31.5">
       <c r="O6" s="3" t="s">
         <v>28</v>
       </c>
@@ -5405,7 +5447,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="15:25" ht="17">
+    <row r="7" spans="15:25">
       <c r="O7" s="6" t="s">
         <v>29</v>
       </c>
@@ -5429,7 +5471,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="15:25" ht="17">
+    <row r="8" spans="15:25">
       <c r="O8" s="6" t="s">
         <v>30</v>
       </c>
@@ -5477,7 +5519,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="15:25" ht="17">
+    <row r="10" spans="15:25">
       <c r="O10" s="6" t="s">
         <v>32</v>
       </c>
@@ -5501,7 +5543,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="15:25" ht="34">
+    <row r="11" spans="15:25">
       <c r="O11" s="6" t="s">
         <v>33</v>
       </c>
@@ -5525,7 +5567,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="15:25" ht="17">
+    <row r="12" spans="15:25">
       <c r="O12" s="6" t="s">
         <v>34</v>
       </c>
@@ -5549,7 +5591,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="15:25" ht="17">
+    <row r="13" spans="15:25">
       <c r="O13" s="6" t="s">
         <v>35</v>
       </c>
@@ -5573,7 +5615,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="15:25" ht="17">
+    <row r="14" spans="15:25">
       <c r="O14" s="6" t="s">
         <v>36</v>
       </c>
@@ -5593,7 +5635,7 @@
       </c>
       <c r="Y14" s="58"/>
     </row>
-    <row r="15" spans="15:25" ht="17">
+    <row r="15" spans="15:25">
       <c r="O15" s="6" t="s">
         <v>37</v>
       </c>
@@ -5617,7 +5659,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="15:25" ht="17">
+    <row r="16" spans="15:25">
       <c r="O16" s="6" t="s">
         <v>38</v>
       </c>
@@ -5641,7 +5683,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="15:25" ht="17">
+    <row r="17" spans="15:25">
       <c r="O17" s="6" t="s">
         <v>39</v>
       </c>
@@ -5665,7 +5707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="15:25" ht="17">
+    <row r="18" spans="15:25">
       <c r="O18" s="6" t="s">
         <v>40</v>
       </c>
@@ -5689,7 +5731,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="15:25" ht="17">
+    <row r="19" spans="15:25">
       <c r="O19" s="6" t="s">
         <v>41</v>
       </c>
@@ -5713,7 +5755,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="15:25" ht="17">
+    <row r="20" spans="15:25">
       <c r="O20" s="6" t="s">
         <v>42</v>
       </c>
@@ -5737,7 +5779,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="15:25" ht="17">
+    <row r="21" spans="15:25">
       <c r="O21" s="6" t="s">
         <v>43</v>
       </c>
@@ -5761,7 +5803,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="15:25" ht="34">
+    <row r="22" spans="15:25">
       <c r="O22" s="6" t="s">
         <v>44</v>
       </c>
@@ -5785,7 +5827,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="15:25" ht="17">
+    <row r="23" spans="15:25">
       <c r="O23" s="6" t="s">
         <v>45</v>
       </c>
@@ -5812,7 +5854,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="15:25" ht="17">
+    <row r="24" spans="15:25">
       <c r="O24" s="6" t="s">
         <v>46</v>
       </c>
@@ -5836,7 +5878,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="15:25" ht="17">
+    <row r="25" spans="15:25">
       <c r="O25" s="6" t="s">
         <v>47</v>
       </c>
@@ -5860,7 +5902,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="15:25" ht="17">
+    <row r="26" spans="15:25">
       <c r="O26" s="6" t="s">
         <v>48</v>
       </c>
@@ -5884,7 +5926,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="15:25" ht="34">
+    <row r="27" spans="15:25">
       <c r="O27" s="6" t="s">
         <v>49</v>
       </c>
@@ -5908,7 +5950,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="15:25" ht="17">
+    <row r="28" spans="15:25">
       <c r="O28" s="6" t="s">
         <v>50</v>
       </c>
@@ -5932,7 +5974,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="15:25" ht="17">
+    <row r="29" spans="15:25">
       <c r="O29" s="6" t="s">
         <v>51</v>
       </c>
@@ -5956,7 +5998,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="15:25" ht="17">
+    <row r="30" spans="15:25">
       <c r="O30" s="6" t="s">
         <v>52</v>
       </c>
@@ -5980,7 +6022,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="15:25" ht="17">
+    <row r="31" spans="15:25">
       <c r="O31" s="6" t="s">
         <v>53</v>
       </c>
@@ -6004,7 +6046,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="15:25" ht="17">
+    <row r="32" spans="15:25">
       <c r="O32" s="6" t="s">
         <v>54</v>
       </c>
@@ -6028,7 +6070,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="15:25" ht="18" thickBot="1">
+    <row r="33" spans="15:25" ht="16.5" thickBot="1">
       <c r="O33" s="18" t="s">
         <v>55</v>
       </c>
@@ -6043,7 +6085,7 @@
     <row r="34" spans="15:25">
       <c r="Y34" s="80"/>
     </row>
-    <row r="37" spans="15:25" ht="17">
+    <row r="37" spans="15:25">
       <c r="U37" s="75" t="s">
         <v>287</v>
       </c>
@@ -6054,7 +6096,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="47" spans="15:25" ht="17" thickBot="1">
+    <row r="47" spans="15:25" ht="16.5" thickBot="1">
       <c r="V47" s="57" t="s">
         <v>83</v>
       </c>
@@ -6100,7 +6142,7 @@
       </c>
       <c r="W53" s="53"/>
     </row>
-    <row r="54" spans="17:23" ht="18" thickBot="1">
+    <row r="54" spans="17:23" ht="16.5" thickBot="1">
       <c r="Q54" s="56" t="s">
         <v>145</v>
       </c>
@@ -6110,7 +6152,7 @@
       <c r="S54" s="26"/>
       <c r="T54" s="26"/>
     </row>
-    <row r="55" spans="17:23" ht="17">
+    <row r="55" spans="17:23">
       <c r="Q55" s="47" t="s">
         <v>72</v>
       </c>
@@ -6120,7 +6162,7 @@
       <c r="S55" s="26"/>
       <c r="T55" s="26"/>
     </row>
-    <row r="56" spans="17:23" ht="17">
+    <row r="56" spans="17:23">
       <c r="Q56" s="50" t="s">
         <v>76</v>
       </c>
@@ -6130,7 +6172,7 @@
       <c r="S56" s="26"/>
       <c r="T56" s="26"/>
     </row>
-    <row r="57" spans="17:23" ht="17">
+    <row r="57" spans="17:23">
       <c r="Q57" s="50" t="s">
         <v>81</v>
       </c>
@@ -6140,7 +6182,7 @@
       <c r="S57" s="26"/>
       <c r="T57" s="26"/>
     </row>
-    <row r="58" spans="17:23" ht="17">
+    <row r="58" spans="17:23">
       <c r="Q58" s="50" t="s">
         <v>84</v>
       </c>
@@ -6150,7 +6192,7 @@
       <c r="S58" s="26"/>
       <c r="T58" s="26"/>
     </row>
-    <row r="59" spans="17:23" ht="17">
+    <row r="59" spans="17:23">
       <c r="Q59" s="50" t="s">
         <v>86</v>
       </c>
@@ -6160,7 +6202,7 @@
       <c r="S59" s="26"/>
       <c r="T59" s="26"/>
     </row>
-    <row r="60" spans="17:23" ht="17">
+    <row r="60" spans="17:23">
       <c r="Q60" s="50" t="s">
         <v>88</v>
       </c>
@@ -6172,15 +6214,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V48" r:id="rId1" xr:uid="{09CCAFCD-4D3B-1B4D-BF48-13B785EDAC17}"/>
-    <hyperlink ref="V49" r:id="rId2" xr:uid="{670087F7-7982-BF43-B2F2-72CACCEA2186}"/>
-    <hyperlink ref="V50" r:id="rId3" xr:uid="{84FC498B-2802-6C49-A607-87D6B590A04F}"/>
-    <hyperlink ref="V52" r:id="rId4" xr:uid="{BA6C3F85-7A32-4242-B7BE-EE9472D0F65F}"/>
-    <hyperlink ref="W48" r:id="rId5" xr:uid="{436812AD-A72D-CF4A-BD02-50C456602ED1}"/>
-    <hyperlink ref="W49" r:id="rId6" xr:uid="{8620EBB2-6F2A-FB45-857E-D330345EF938}"/>
-    <hyperlink ref="V51" r:id="rId7" xr:uid="{97B05C91-91FA-4749-867E-A9E2FE16DE57}"/>
-    <hyperlink ref="V53" r:id="rId8" xr:uid="{D3AEC8A1-0926-0040-A9E7-F6A53E499A03}"/>
-    <hyperlink ref="V47" r:id="rId9" xr:uid="{1425EEE8-52FF-CB48-805D-78E11BA1BFF7}"/>
+    <hyperlink ref="V48" r:id="rId1"/>
+    <hyperlink ref="V49" r:id="rId2"/>
+    <hyperlink ref="V50" r:id="rId3"/>
+    <hyperlink ref="V52" r:id="rId4"/>
+    <hyperlink ref="W48" r:id="rId5"/>
+    <hyperlink ref="W49" r:id="rId6"/>
+    <hyperlink ref="V51" r:id="rId7"/>
+    <hyperlink ref="V53" r:id="rId8"/>
+    <hyperlink ref="V47" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>